<commit_message>
Adding snw on the day table. Inserting the Eday table with mrros #707.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/miscellaneous-data-requests/knmi23-dutch-scenarios/cmvme_CMIP_ssp245_1_1-knmi23-plev23r.xlsx
+++ b/ece2cmor3/resources/miscellaneous-data-requests/knmi23-dutch-scenarios/cmvme_CMIP_ssp245_1_1-knmi23-plev23r.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,8 +27,9 @@
     <sheet name="Oyr" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="SIday" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="SImon" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="day" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="fx" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Eday" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="day" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="fx" sheetId="22" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1625,6 +1626,128 @@
 </comments>
 </file>
 
+<file path=xl/comments22.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Lowest priority value set in request for this variable for this experiment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">NetCDF Global Attribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Name of variable in file</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">CMOR directive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">CMOR name, unique within table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">CMOR variable identifier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">MIP variable identifier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Structure identifier</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
@@ -2480,7 +2603,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10891" uniqueCount="3225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10925" uniqueCount="3225">
   <si>
     <t xml:space="preserve">Notes on tables</t>
   </si>
@@ -12354,7 +12477,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12557,7 +12680,7 @@
   <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13387,7 +13510,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14739,7 +14862,7 @@
   <dimension ref="A1:AF54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19107,7 +19230,7 @@
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19469,7 +19592,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19677,7 +19800,7 @@
   <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20514,8 +20637,8 @@
   </sheetPr>
   <dimension ref="A1:AF129"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA129" activeCellId="0" sqref="AA129"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA129" activeCellId="1" sqref="1:2 AA129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30942,7 +31065,7 @@
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33326,7 +33449,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33618,7 +33741,7 @@
   <dimension ref="A1:AF40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB40" activeCellId="0" sqref="AB40"/>
+      <selection pane="topLeft" activeCell="AB40" activeCellId="1" sqref="1:2 AB40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36763,7 +36886,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36901,10 +37024,138 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB31" activeCellId="0" sqref="AB31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="0" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AF32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L32" activeCellId="1" sqref="1:2 L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39401,6 +39652,11 @@
       </c>
       <c r="AB31" s="0" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L32" s="0" t="s">
+        <v>1201</v>
       </c>
     </row>
   </sheetData>
@@ -39415,7 +39671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -39423,7 +39679,7 @@
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="1" sqref="1:2 L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40211,7 +40467,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40348,7 +40604,7 @@
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="1:2 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40552,7 +40808,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40842,7 +41098,7 @@
   <dimension ref="A1:AF76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -47414,7 +47670,7 @@
   <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48214,7 +48470,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -48502,7 +48758,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>